<commit_message>
Optimize code log and reconfigure issue statistics to send email time
</commit_message>
<xml_diff>
--- a/cve-py/issue_statistics/to_email.xlsx
+++ b/cve-py/issue_statistics/to_email.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView windowWidth="28650" windowHeight="11355"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>name</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>zhangjianjun21@huawei.com</t>
+  </si>
+  <si>
+    <t>jjzhangcm@isoftstone.com</t>
   </si>
 </sst>
 </file>
@@ -58,21 +61,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -94,23 +99,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -124,6 +113,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,7 +166,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -166,28 +191,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -202,37 +205,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -244,73 +367,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,61 +379,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,30 +396,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -431,6 +410,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -479,16 +482,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -501,10 +504,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -513,16 +516,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -531,115 +534,115 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -998,13 +1001,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
   </cols>
@@ -1033,10 +1036,19 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="guoxiaoqi2@huawei.com"/>
     <hyperlink ref="A3" r:id="rId2" display="zhangjianjun21@huawei.com"/>
+    <hyperlink ref="A4" r:id="rId3" display="jjzhangcm@isoftstone.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Generate cvrf data repair; update the issue statistics mailing list
</commit_message>
<xml_diff>
--- a/cve-py/issue_statistics/to_email.xlsx
+++ b/cve-py/issue_statistics/to_email.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>name</t>
   </si>
@@ -24,13 +24,94 @@
     <t>type</t>
   </si>
   <si>
+    <t>liujingang09@huawei.com</t>
+  </si>
+  <si>
+    <t>solar.hu@huawei.com</t>
+  </si>
+  <si>
+    <t>chenyaqiang@huawei.com</t>
+  </si>
+  <si>
+    <t>alex.chen@huawei.com</t>
+  </si>
+  <si>
+    <t>xiexiuqi@huawei.com</t>
+  </si>
+  <si>
+    <t>xiasenlin1@huawei.com</t>
+  </si>
+  <si>
+    <t>fanjiachen3@huawei.com</t>
+  </si>
+  <si>
+    <t>yangyingliang@huawei.com</t>
+  </si>
+  <si>
+    <t>songnannan2@huawei.com</t>
+  </si>
+  <si>
+    <t>shenyangyang4@huawei.com</t>
+  </si>
+  <si>
+    <t>lijiajie11@huawei.com</t>
+  </si>
+  <si>
     <t>guoxiaoqi2@huawei.com</t>
   </si>
   <si>
     <t>zhangjianjun21@huawei.com</t>
   </si>
   <si>
-    <t>jjzhangcm@isoftstone.com</t>
+    <t>zhujianwei7@huawei.com</t>
+  </si>
+  <si>
+    <t>yanglijin@huawei.com</t>
+  </si>
+  <si>
+    <t>y69393@huawei.com</t>
+  </si>
+  <si>
+    <t>yanxiaobing@huawei.com</t>
+  </si>
+  <si>
+    <t>weigang12@huawei.com</t>
+  </si>
+  <si>
+    <t>huxinwei@huawei.com</t>
+  </si>
+  <si>
+    <t>xiongwei888@huawei.com</t>
+  </si>
+  <si>
+    <t>zhenhua.jiang@huawei.com</t>
+  </si>
+  <si>
+    <t>jiangyumin@huawei.com</t>
+  </si>
+  <si>
+    <t>zhuyanpeng@huawei.com</t>
+  </si>
+  <si>
+    <t>wangyiru1@huawei.com</t>
+  </si>
+  <si>
+    <t>zhuyuncheng@huawei.com</t>
+  </si>
+  <si>
+    <t>luoshengwei@huawei.com</t>
+  </si>
+  <si>
+    <t>yangyunyi2@huawei.com</t>
+  </si>
+  <si>
+    <t>lihaiwei8@huawei.com</t>
+  </si>
+  <si>
+    <t>tushenmei@huawei.com</t>
+  </si>
+  <si>
+    <t>huangzhuo11@huawei.com</t>
   </si>
 </sst>
 </file>
@@ -38,10 +119,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -60,6 +141,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -67,17 +156,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -91,6 +187,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
@@ -99,7 +225,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -114,83 +263,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,37 +286,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,13 +424,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,43 +448,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,79 +466,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -396,6 +477,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -410,21 +502,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -455,11 +532,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -469,15 +559,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -504,10 +585,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -516,16 +597,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -534,123 +615,126 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1001,13 +1085,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
   </cols>
@@ -1044,11 +1128,254 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="guoxiaoqi2@huawei.com"/>
-    <hyperlink ref="A3" r:id="rId2" display="zhangjianjun21@huawei.com"/>
-    <hyperlink ref="A4" r:id="rId3" display="jjzhangcm@isoftstone.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="liujingang09@huawei.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="solar.hu@huawei.com"/>
+    <hyperlink ref="A4" r:id="rId3" display="chenyaqiang@huawei.com"/>
+    <hyperlink ref="A5" r:id="rId4" display="alex.chen@huawei.com" tooltip="mailto:alex.chen@huawei.com"/>
+    <hyperlink ref="A6" r:id="rId5" display="xiexiuqi@huawei.com"/>
+    <hyperlink ref="A7" r:id="rId6" display="xiasenlin1@huawei.com"/>
+    <hyperlink ref="A8" r:id="rId7" display="fanjiachen3@huawei.com"/>
+    <hyperlink ref="A9" r:id="rId8" display="yangyingliang@huawei.com"/>
+    <hyperlink ref="A10" r:id="rId9" display="songnannan2@huawei.com"/>
+    <hyperlink ref="A11" r:id="rId10" display="shenyangyang4@huawei.com"/>
+    <hyperlink ref="A12" r:id="rId11" display="lijiajie11@huawei.com"/>
+    <hyperlink ref="A13" r:id="rId12" display="guoxiaoqi2@huawei.com"/>
+    <hyperlink ref="A14" r:id="rId13" display="zhangjianjun21@huawei.com"/>
+    <hyperlink ref="A15" r:id="rId14" display="zhujianwei7@huawei.com"/>
+    <hyperlink ref="A16" r:id="rId15" display="yanglijin@huawei.com"/>
+    <hyperlink ref="A17" r:id="rId16" display="y69393@huawei.com"/>
+    <hyperlink ref="A18" r:id="rId17" display="yanxiaobing@huawei.com"/>
+    <hyperlink ref="A19" r:id="rId18" display="weigang12@huawei.com"/>
+    <hyperlink ref="A20" r:id="rId19" display="huxinwei@huawei.com"/>
+    <hyperlink ref="A21" r:id="rId20" display="xiongwei888@huawei.com"/>
+    <hyperlink ref="A22" r:id="rId21" display="zhenhua.jiang@huawei.com" tooltip="mailto:zhenhua.jiang@huawei.com"/>
+    <hyperlink ref="A23" r:id="rId22" display="jiangyumin@huawei.com"/>
+    <hyperlink ref="A24" r:id="rId23" display="zhuyanpeng@huawei.com"/>
+    <hyperlink ref="A25" r:id="rId24" display="wangyiru1@huawei.com"/>
+    <hyperlink ref="A26" r:id="rId25" display="zhuyuncheng@huawei.com"/>
+    <hyperlink ref="A27" r:id="rId26" display="luoshengwei@huawei.com" tooltip="mailto:luoshengwei@huawei.com"/>
+    <hyperlink ref="A28" r:id="rId27" display="yangyunyi2@huawei.com"/>
+    <hyperlink ref="A30" r:id="rId28" display="tushenmei@huawei.com"/>
+    <hyperlink ref="A31" r:id="rId29" display="huangzhuo11@huawei.com"/>
+    <hyperlink ref="A29" r:id="rId30" display="lihaiwei8@huawei.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
1. Added statistics on senders of issue emails; 2. Code optimization
</commit_message>
<xml_diff>
--- a/cve-py/issue_statistics/to_email.xlsx
+++ b/cve-py/issue_statistics/to_email.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>name</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>guoxiaoqi2@huawei.com</t>
+  </si>
+  <si>
+    <t>liyongqiang10@huawei.com</t>
+  </si>
+  <si>
+    <t>wangyue92@huawei.com</t>
   </si>
   <si>
     <t>zhangjianjun21@huawei.com</t>
@@ -119,10 +125,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -149,6 +155,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -163,17 +199,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -196,7 +254,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,74 +262,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,12 +292,90 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -304,7 +388,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -316,157 +466,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,17 +483,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -508,8 +503,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -533,8 +530,41 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -553,30 +583,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -585,10 +591,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -597,16 +603,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -618,112 +624,112 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1085,10 +1091,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
@@ -1213,7 +1219,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1221,7 +1227,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1265,7 +1271,7 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B22">
@@ -1281,7 +1287,7 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B24">
@@ -1341,6 +1347,22 @@
         <v>31</v>
       </c>
       <c r="B31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
         <v>2</v>
       </c>
     </row>
@@ -1358,24 +1380,26 @@
     <hyperlink ref="A11" r:id="rId10" display="shenyangyang4@huawei.com"/>
     <hyperlink ref="A12" r:id="rId11" display="lijiajie11@huawei.com"/>
     <hyperlink ref="A13" r:id="rId12" display="guoxiaoqi2@huawei.com"/>
-    <hyperlink ref="A14" r:id="rId13" display="zhangjianjun21@huawei.com"/>
-    <hyperlink ref="A15" r:id="rId14" display="zhujianwei7@huawei.com"/>
-    <hyperlink ref="A16" r:id="rId15" display="yanglijin@huawei.com"/>
-    <hyperlink ref="A17" r:id="rId16" display="y69393@huawei.com"/>
-    <hyperlink ref="A18" r:id="rId17" display="yanxiaobing@huawei.com"/>
-    <hyperlink ref="A19" r:id="rId18" display="weigang12@huawei.com"/>
-    <hyperlink ref="A20" r:id="rId19" display="huxinwei@huawei.com"/>
-    <hyperlink ref="A21" r:id="rId20" display="xiongwei888@huawei.com"/>
-    <hyperlink ref="A22" r:id="rId21" display="zhenhua.jiang@huawei.com" tooltip="mailto:zhenhua.jiang@huawei.com"/>
-    <hyperlink ref="A23" r:id="rId22" display="jiangyumin@huawei.com"/>
-    <hyperlink ref="A24" r:id="rId23" display="zhuyanpeng@huawei.com"/>
-    <hyperlink ref="A25" r:id="rId24" display="wangyiru1@huawei.com"/>
-    <hyperlink ref="A26" r:id="rId25" display="zhuyuncheng@huawei.com"/>
-    <hyperlink ref="A27" r:id="rId26" display="luoshengwei@huawei.com" tooltip="mailto:luoshengwei@huawei.com"/>
-    <hyperlink ref="A28" r:id="rId27" display="yangyunyi2@huawei.com"/>
-    <hyperlink ref="A30" r:id="rId28" display="tushenmei@huawei.com"/>
-    <hyperlink ref="A31" r:id="rId29" display="huangzhuo11@huawei.com"/>
-    <hyperlink ref="A29" r:id="rId30" display="lihaiwei8@huawei.com"/>
+    <hyperlink ref="A16" r:id="rId13" display="zhangjianjun21@huawei.com"/>
+    <hyperlink ref="A17" r:id="rId14" display="zhujianwei7@huawei.com"/>
+    <hyperlink ref="A18" r:id="rId15" display="yanglijin@huawei.com"/>
+    <hyperlink ref="A19" r:id="rId16" display="y69393@huawei.com"/>
+    <hyperlink ref="A20" r:id="rId17" display="yanxiaobing@huawei.com"/>
+    <hyperlink ref="A21" r:id="rId18" display="weigang12@huawei.com"/>
+    <hyperlink ref="A22" r:id="rId19" display="huxinwei@huawei.com"/>
+    <hyperlink ref="A23" r:id="rId20" display="xiongwei888@huawei.com"/>
+    <hyperlink ref="A24" r:id="rId21" display="zhenhua.jiang@huawei.com" tooltip="mailto:zhenhua.jiang@huawei.com"/>
+    <hyperlink ref="A25" r:id="rId22" display="jiangyumin@huawei.com"/>
+    <hyperlink ref="A26" r:id="rId23" display="zhuyanpeng@huawei.com"/>
+    <hyperlink ref="A27" r:id="rId24" display="wangyiru1@huawei.com"/>
+    <hyperlink ref="A28" r:id="rId25" display="zhuyuncheng@huawei.com"/>
+    <hyperlink ref="A29" r:id="rId26" display="luoshengwei@huawei.com" tooltip="mailto:luoshengwei@huawei.com"/>
+    <hyperlink ref="A30" r:id="rId27" display="yangyunyi2@huawei.com"/>
+    <hyperlink ref="A32" r:id="rId28" display="tushenmei@huawei.com"/>
+    <hyperlink ref="A33" r:id="rId29" display="huangzhuo11@huawei.com"/>
+    <hyperlink ref="A31" r:id="rId30" display="lihaiwei8@huawei.com"/>
+    <hyperlink ref="A15" r:id="rId31" display="wangyue92@huawei.com"/>
+    <hyperlink ref="A14" r:id="rId32" display="liyongqiang10@huawei.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Modify the yaml file download link
</commit_message>
<xml_diff>
--- a/cve-py/issue_statistics/to_email.xlsx
+++ b/cve-py/issue_statistics/to_email.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>zhujunhao8@huawei.com</t>
+  </si>
+  <si>
+    <t>shanzhikun@huawei.com</t>
   </si>
   <si>
     <t>wangyue92@huawei.com</t>
@@ -129,9 +132,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -159,19 +162,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -195,7 +199,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -210,7 +245,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,24 +253,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -247,40 +267,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -295,6 +298,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -307,175 +364,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,11 +492,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,6 +511,17 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -524,20 +544,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,17 +566,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -594,10 +597,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -606,16 +609,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -627,112 +630,112 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1094,10 +1097,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
@@ -1226,7 +1229,7 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16">
@@ -1234,7 +1237,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B17">
@@ -1246,7 +1249,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1298,7 +1301,7 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B25">
@@ -1306,7 +1309,7 @@
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B26">
@@ -1374,6 +1377,14 @@
         <v>34</v>
       </c>
       <c r="B34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
         <v>2</v>
       </c>
     </row>
@@ -1391,27 +1402,28 @@
     <hyperlink ref="A11" r:id="rId10" display="shenyangyang4@huawei.com"/>
     <hyperlink ref="A12" r:id="rId11" display="lijiajie11@huawei.com"/>
     <hyperlink ref="A13" r:id="rId12" display="guoxiaoqi2@huawei.com"/>
-    <hyperlink ref="A17" r:id="rId13" display="zhangjianjun21@huawei.com"/>
-    <hyperlink ref="A18" r:id="rId14" display="zhujianwei7@huawei.com"/>
-    <hyperlink ref="A19" r:id="rId15" display="yanglijin@huawei.com"/>
-    <hyperlink ref="A20" r:id="rId16" display="y69393@huawei.com"/>
-    <hyperlink ref="A21" r:id="rId17" display="yanxiaobing@huawei.com"/>
-    <hyperlink ref="A22" r:id="rId18" display="weigang12@huawei.com"/>
-    <hyperlink ref="A23" r:id="rId19" display="huxinwei@huawei.com"/>
-    <hyperlink ref="A24" r:id="rId20" display="xiongwei888@huawei.com"/>
-    <hyperlink ref="A25" r:id="rId21" display="zhenhua.jiang@huawei.com" tooltip="mailto:zhenhua.jiang@huawei.com"/>
-    <hyperlink ref="A26" r:id="rId22" display="jiangyumin@huawei.com"/>
-    <hyperlink ref="A27" r:id="rId23" display="zhuyanpeng@huawei.com"/>
-    <hyperlink ref="A28" r:id="rId24" display="wangyiru1@huawei.com"/>
-    <hyperlink ref="A29" r:id="rId25" display="zhuyuncheng@huawei.com"/>
-    <hyperlink ref="A30" r:id="rId26" display="luoshengwei@huawei.com" tooltip="mailto:luoshengwei@huawei.com"/>
-    <hyperlink ref="A31" r:id="rId27" display="yangyunyi2@huawei.com"/>
-    <hyperlink ref="A33" r:id="rId28" display="tushenmei@huawei.com"/>
-    <hyperlink ref="A34" r:id="rId29" display="huangzhuo11@huawei.com"/>
-    <hyperlink ref="A32" r:id="rId30" display="lihaiwei8@huawei.com"/>
-    <hyperlink ref="A16" r:id="rId31" display="wangyue92@huawei.com"/>
+    <hyperlink ref="A18" r:id="rId13" display="zhangjianjun21@huawei.com"/>
+    <hyperlink ref="A19" r:id="rId14" display="zhujianwei7@huawei.com"/>
+    <hyperlink ref="A20" r:id="rId15" display="yanglijin@huawei.com"/>
+    <hyperlink ref="A21" r:id="rId16" display="y69393@huawei.com"/>
+    <hyperlink ref="A22" r:id="rId17" display="yanxiaobing@huawei.com"/>
+    <hyperlink ref="A23" r:id="rId18" display="weigang12@huawei.com"/>
+    <hyperlink ref="A24" r:id="rId19" display="huxinwei@huawei.com"/>
+    <hyperlink ref="A25" r:id="rId20" display="xiongwei888@huawei.com"/>
+    <hyperlink ref="A26" r:id="rId21" display="zhenhua.jiang@huawei.com" tooltip="mailto:zhenhua.jiang@huawei.com"/>
+    <hyperlink ref="A27" r:id="rId22" display="jiangyumin@huawei.com"/>
+    <hyperlink ref="A28" r:id="rId23" display="zhuyanpeng@huawei.com"/>
+    <hyperlink ref="A29" r:id="rId24" display="wangyiru1@huawei.com"/>
+    <hyperlink ref="A30" r:id="rId25" display="zhuyuncheng@huawei.com"/>
+    <hyperlink ref="A31" r:id="rId26" display="luoshengwei@huawei.com" tooltip="mailto:luoshengwei@huawei.com"/>
+    <hyperlink ref="A32" r:id="rId27" display="yangyunyi2@huawei.com"/>
+    <hyperlink ref="A34" r:id="rId28" display="tushenmei@huawei.com"/>
+    <hyperlink ref="A35" r:id="rId29" display="huangzhuo11@huawei.com"/>
+    <hyperlink ref="A33" r:id="rId30" display="lihaiwei8@huawei.com"/>
+    <hyperlink ref="A17" r:id="rId31" display="wangyue92@huawei.com"/>
     <hyperlink ref="A14" r:id="rId32" display="liyongqiang10@huawei.com"/>
     <hyperlink ref="A15" r:id="rId33" display="zhujunhao8@huawei.com"/>
+    <hyperlink ref="A16" r:id="rId34" display="shanzhikun@huawei.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>